<commit_message>
Uploading new URDF, IK, Solidworks file
</commit_message>
<xml_diff>
--- a/Excel Files/Purchase items.xlsx
+++ b/Excel Files/Purchase items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EMGingers-control\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505073A4-14A7-432E-B76E-6D7524E764DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3233FA-7799-4FD6-B867-3221D5D29F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>No</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Servo Cables</t>
+  </si>
+  <si>
+    <t>XT60</t>
+  </si>
+  <si>
+    <t>EC5</t>
+  </si>
+  <si>
+    <t>Pro Mini</t>
   </si>
 </sst>
 </file>
@@ -381,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D10"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +433,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>41.55</v>
+        <v>69.69</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -483,9 +492,42 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D10" s="1">
-        <f>SUM(D3:D9)</f>
-        <v>163.01999999999998</v>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D13" s="1">
+        <f>SUM(D3:D12)</f>
+        <v>204.69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>